<commit_message>
Modified .xlsx outputs files to better reading and added location text. Code also added in .py file
</commit_message>
<xml_diff>
--- a/listados/pedidos.xlsx
+++ b/listados/pedidos.xlsx
@@ -111,7 +111,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +140,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -161,17 +168,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,364 +480,364 @@
   <sheetData>
     <row r="1" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
+      <c r="D1" s="2"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="2"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
+      <c r="B3" s="5"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="5" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="5" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="5" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="5" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="5" t="s">
+      <c r="B17" s="5"/>
+      <c r="C17" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="5" t="s">
+      <c r="B18" s="5"/>
+      <c r="C18" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="5" t="s">
+      <c r="B19" s="5"/>
+      <c r="C19" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="5" t="s">
+      <c r="B20" s="5"/>
+      <c r="C20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="5" t="s">
+      <c r="B21" s="5"/>
+      <c r="C21" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="5" t="s">
+      <c r="B22" s="5"/>
+      <c r="C22" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="4"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="5" t="s">
+      <c r="B24" s="5"/>
+      <c r="C24" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="4"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="5" t="s">
+      <c r="B26" s="5"/>
+      <c r="C26" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="5" t="s">
+      <c r="B27" s="5"/>
+      <c r="C27" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="4"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="4"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
       <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="5" t="s">
+      <c r="B30" s="5"/>
+      <c r="C30" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="5" t="s">
+      <c r="B31" s="5"/>
+      <c r="C31" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Final version. Has suc_names in the .xls files and can create files from same sucursal with different oc. Tested and .exe created
</commit_message>
<xml_diff>
--- a/listados/pedidos.xlsx
+++ b/listados/pedidos.xlsx
@@ -168,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -180,6 +180,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,7 +465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -478,7 +481,7 @@
     <col min="8" max="8" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="5"/>
       <c r="C1" s="3" t="s">
@@ -486,7 +489,7 @@
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="6"/>
+      <c r="F1" s="7"/>
       <c r="G1" s="6"/>
       <c r="H1" s="1"/>
     </row>

</xml_diff>